<commit_message>
Upload Y4_B2526_General_&_special_internal_1_schedule.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/modules_schedules/Y4_B2526_General_&_special_internal_1_schedule.xlsx
+++ b/modules_schedules/Y4_B2526_General_&_special_internal_1_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\modules_schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EF0778-033A-48C5-AA7A-0032F9D7ED9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E03F083-D1AF-4A0D-9AB2-96670B110ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="90">
   <si>
     <t>Year</t>
   </si>
@@ -262,33 +262,6 @@
     <t>B1B</t>
   </si>
   <si>
-    <t>20/9/2025</t>
-  </si>
-  <si>
-    <t>21/9/2025</t>
-  </si>
-  <si>
-    <t>22/9/2025</t>
-  </si>
-  <si>
-    <t>23/9/2025</t>
-  </si>
-  <si>
-    <t>24/9/2025</t>
-  </si>
-  <si>
-    <t>27/9/2025</t>
-  </si>
-  <si>
-    <t>28/9/2025</t>
-  </si>
-  <si>
-    <t>29/9/2025</t>
-  </si>
-  <si>
-    <t>30/9/2025</t>
-  </si>
-  <si>
     <t>16/10/2025</t>
   </si>
   <si>
@@ -299,9 +272,6 @@
   </si>
   <si>
     <t>13/09/2025</t>
-  </si>
-  <si>
-    <t>25/9/2025</t>
   </si>
   <si>
     <t>B1D</t>
@@ -710,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
-      <selection activeCell="A254" sqref="A254:XFD254"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2001,8 +1971,8 @@
       <c r="D56" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E56" s="7" t="s">
-        <v>80</v>
+      <c r="E56" s="7">
+        <v>45920</v>
       </c>
       <c r="F56" s="8" t="s">
         <v>12</v>
@@ -2024,8 +1994,8 @@
       <c r="D57" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>81</v>
+      <c r="E57" s="3">
+        <v>45921</v>
       </c>
       <c r="F57" s="4" t="s">
         <v>12</v>
@@ -2047,8 +2017,8 @@
       <c r="D58" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E58" s="7" t="s">
-        <v>82</v>
+      <c r="E58" s="7">
+        <v>45922</v>
       </c>
       <c r="F58" s="8" t="s">
         <v>12</v>
@@ -2070,8 +2040,8 @@
       <c r="D59" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="3" t="s">
-        <v>83</v>
+      <c r="E59" s="3">
+        <v>45923</v>
       </c>
       <c r="F59" s="4" t="s">
         <v>12</v>
@@ -2093,8 +2063,8 @@
       <c r="D60" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E60" s="7" t="s">
-        <v>84</v>
+      <c r="E60" s="7">
+        <v>45924</v>
       </c>
       <c r="F60" s="8" t="s">
         <v>12</v>
@@ -2116,8 +2086,8 @@
       <c r="D61" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E61" s="3" t="s">
-        <v>85</v>
+      <c r="E61" s="3">
+        <v>45927</v>
       </c>
       <c r="F61" s="4" t="s">
         <v>12</v>
@@ -2139,8 +2109,8 @@
       <c r="D62" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E62" s="7" t="s">
-        <v>86</v>
+      <c r="E62" s="7">
+        <v>45928</v>
       </c>
       <c r="F62" s="8" t="s">
         <v>12</v>
@@ -2162,8 +2132,8 @@
       <c r="D63" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E63" s="3" t="s">
-        <v>87</v>
+      <c r="E63" s="3">
+        <v>45929</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>12</v>
@@ -2185,8 +2155,8 @@
       <c r="D64" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E64" s="7" t="s">
-        <v>88</v>
+      <c r="E64" s="7">
+        <v>45930</v>
       </c>
       <c r="F64" s="8" t="s">
         <v>12</v>
@@ -2416,7 +2386,7 @@
         <v>29</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F74" s="8" t="s">
         <v>12</v>
@@ -3212,7 +3182,7 @@
         <v>7</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C109" s="6" t="s">
         <v>9</v>
@@ -3221,7 +3191,7 @@
         <v>10</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F109" s="8" t="s">
         <v>12</v>
@@ -3235,7 +3205,7 @@
         <v>7</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>9</v>
@@ -3258,7 +3228,7 @@
         <v>7</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>9</v>
@@ -3281,7 +3251,7 @@
         <v>7</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>9</v>
@@ -3304,7 +3274,7 @@
         <v>7</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>9</v>
@@ -3327,7 +3297,7 @@
         <v>7</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>9</v>
@@ -3336,7 +3306,7 @@
         <v>21</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F114" s="4" t="s">
         <v>12</v>
@@ -3350,7 +3320,7 @@
         <v>7</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C115" s="6" t="s">
         <v>9</v>
@@ -3373,7 +3343,7 @@
         <v>7</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>9</v>
@@ -3396,7 +3366,7 @@
         <v>7</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C117" s="6" t="s">
         <v>9</v>
@@ -3419,7 +3389,7 @@
         <v>7</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>9</v>
@@ -3442,7 +3412,7 @@
         <v>7</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C119" s="6" t="s">
         <v>31</v>
@@ -3450,8 +3420,8 @@
       <c r="D119" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E119" s="7" t="s">
-        <v>81</v>
+      <c r="E119" s="7">
+        <v>45921</v>
       </c>
       <c r="F119" s="8" t="s">
         <v>12</v>
@@ -3465,7 +3435,7 @@
         <v>7</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>31</v>
@@ -3473,8 +3443,8 @@
       <c r="D120" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E120" s="3" t="s">
-        <v>82</v>
+      <c r="E120" s="3">
+        <v>45922</v>
       </c>
       <c r="F120" s="4" t="s">
         <v>12</v>
@@ -3488,7 +3458,7 @@
         <v>7</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>31</v>
@@ -3496,8 +3466,8 @@
       <c r="D121" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E121" s="7" t="s">
-        <v>83</v>
+      <c r="E121" s="7">
+        <v>45923</v>
       </c>
       <c r="F121" s="8" t="s">
         <v>12</v>
@@ -3511,7 +3481,7 @@
         <v>7</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>31</v>
@@ -3519,8 +3489,8 @@
       <c r="D122" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E122" s="3" t="s">
-        <v>84</v>
+      <c r="E122" s="3">
+        <v>45924</v>
       </c>
       <c r="F122" s="4" t="s">
         <v>12</v>
@@ -3534,7 +3504,7 @@
         <v>7</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C123" s="6" t="s">
         <v>31</v>
@@ -3542,8 +3512,8 @@
       <c r="D123" s="6">
         <v>5</v>
       </c>
-      <c r="E123" s="7" t="s">
-        <v>93</v>
+      <c r="E123" s="7">
+        <v>45925</v>
       </c>
       <c r="F123" s="8" t="s">
         <v>12</v>
@@ -3557,7 +3527,7 @@
         <v>7</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>31</v>
@@ -3565,8 +3535,8 @@
       <c r="D124" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E124" s="3" t="s">
-        <v>86</v>
+      <c r="E124" s="3">
+        <v>45928</v>
       </c>
       <c r="F124" s="4" t="s">
         <v>12</v>
@@ -3580,7 +3550,7 @@
         <v>7</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C125" s="6" t="s">
         <v>31</v>
@@ -3588,8 +3558,8 @@
       <c r="D125" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E125" s="7" t="s">
-        <v>87</v>
+      <c r="E125" s="7">
+        <v>45929</v>
       </c>
       <c r="F125" s="8" t="s">
         <v>12</v>
@@ -3603,7 +3573,7 @@
         <v>7</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>31</v>
@@ -3611,8 +3581,8 @@
       <c r="D126" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E126" s="3" t="s">
-        <v>88</v>
+      <c r="E126" s="3">
+        <v>45930</v>
       </c>
       <c r="F126" s="4" t="s">
         <v>12</v>
@@ -3626,7 +3596,7 @@
         <v>7</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C127" s="6" t="s">
         <v>31</v>
@@ -3649,7 +3619,7 @@
         <v>7</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>31</v>
@@ -3672,7 +3642,7 @@
         <v>7</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C129" s="6" t="s">
         <v>42</v>
@@ -3695,7 +3665,7 @@
         <v>7</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>42</v>
@@ -3718,7 +3688,7 @@
         <v>7</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C131" s="6" t="s">
         <v>42</v>
@@ -3741,7 +3711,7 @@
         <v>7</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>42</v>
@@ -3764,7 +3734,7 @@
         <v>7</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C133" s="6" t="s">
         <v>42</v>
@@ -3787,7 +3757,7 @@
         <v>7</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>49</v>
@@ -3810,7 +3780,7 @@
         <v>7</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C135" s="6" t="s">
         <v>49</v>
@@ -3833,7 +3803,7 @@
         <v>7</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>49</v>
@@ -3856,7 +3826,7 @@
         <v>7</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C137" s="6" t="s">
         <v>49</v>
@@ -3879,7 +3849,7 @@
         <v>7</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>55</v>
@@ -3902,7 +3872,7 @@
         <v>7</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C139" s="6" t="s">
         <v>55</v>
@@ -3925,7 +3895,7 @@
         <v>7</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>55</v>
@@ -3948,7 +3918,7 @@
         <v>7</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C141" s="6" t="s">
         <v>55</v>
@@ -3971,7 +3941,7 @@
         <v>7</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>55</v>
@@ -3994,7 +3964,7 @@
         <v>7</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C143" s="6" t="s">
         <v>55</v>
@@ -4017,7 +3987,7 @@
         <v>7</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>55</v>
@@ -4040,7 +4010,7 @@
         <v>7</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C145" s="6" t="s">
         <v>55</v>
@@ -4063,7 +4033,7 @@
         <v>7</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>55</v>
@@ -4086,7 +4056,7 @@
         <v>7</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C147" s="6" t="s">
         <v>55</v>
@@ -4109,7 +4079,7 @@
         <v>7</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C148" s="6" t="s">
         <v>62</v>
@@ -4132,7 +4102,7 @@
         <v>7</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>62</v>
@@ -4155,7 +4125,7 @@
         <v>7</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C150" s="6" t="s">
         <v>62</v>
@@ -4178,7 +4148,7 @@
         <v>7</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>62</v>
@@ -4201,7 +4171,7 @@
         <v>7</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C152" s="6" t="s">
         <v>62</v>
@@ -4224,7 +4194,7 @@
         <v>7</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C153" s="2" t="s">
         <v>62</v>
@@ -4247,7 +4217,7 @@
         <v>7</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C154" s="6" t="s">
         <v>62</v>
@@ -4270,7 +4240,7 @@
         <v>7</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C155" s="2" t="s">
         <v>62</v>
@@ -4293,7 +4263,7 @@
         <v>7</v>
       </c>
       <c r="B156" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C156" s="6" t="s">
         <v>62</v>
@@ -4316,7 +4286,7 @@
         <v>7</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>73</v>
@@ -4339,7 +4309,7 @@
         <v>7</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C158" s="6" t="s">
         <v>73</v>
@@ -4362,7 +4332,7 @@
         <v>7</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>73</v>
@@ -4385,7 +4355,7 @@
         <v>7</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C160" s="6" t="s">
         <v>73</v>
@@ -4408,7 +4378,7 @@
         <v>7</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>73</v>
@@ -4417,7 +4387,7 @@
         <v>19</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F161" s="4" t="s">
         <v>12</v>
@@ -4431,7 +4401,7 @@
         <v>7</v>
       </c>
       <c r="B162" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C162" s="6" t="s">
         <v>9</v>
@@ -4440,7 +4410,7 @@
         <v>10</v>
       </c>
       <c r="E162" s="7" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F162" s="8" t="s">
         <v>12</v>
@@ -4454,7 +4424,7 @@
         <v>7</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C163" s="2" t="s">
         <v>9</v>
@@ -4477,7 +4447,7 @@
         <v>7</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C164" s="6" t="s">
         <v>9</v>
@@ -4500,7 +4470,7 @@
         <v>7</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>9</v>
@@ -4523,7 +4493,7 @@
         <v>7</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C166" s="6" t="s">
         <v>9</v>
@@ -4546,7 +4516,7 @@
         <v>7</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C167" s="2" t="s">
         <v>9</v>
@@ -4555,7 +4525,7 @@
         <v>21</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F167" s="4" t="s">
         <v>12</v>
@@ -4569,7 +4539,7 @@
         <v>7</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C168" s="6" t="s">
         <v>9</v>
@@ -4592,7 +4562,7 @@
         <v>7</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>9</v>
@@ -4615,7 +4585,7 @@
         <v>7</v>
       </c>
       <c r="B170" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C170" s="6" t="s">
         <v>9</v>
@@ -4638,7 +4608,7 @@
         <v>7</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>9</v>
@@ -4661,7 +4631,7 @@
         <v>7</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C172" s="6" t="s">
         <v>31</v>
@@ -4684,7 +4654,7 @@
         <v>7</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>31</v>
@@ -4707,7 +4677,7 @@
         <v>7</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C174" s="6" t="s">
         <v>31</v>
@@ -4730,7 +4700,7 @@
         <v>7</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>31</v>
@@ -4753,7 +4723,7 @@
         <v>7</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C176" s="6" t="s">
         <v>31</v>
@@ -4776,7 +4746,7 @@
         <v>7</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>31</v>
@@ -4799,7 +4769,7 @@
         <v>7</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C178" s="6" t="s">
         <v>31</v>
@@ -4822,7 +4792,7 @@
         <v>7</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C179" s="2" t="s">
         <v>31</v>
@@ -4845,7 +4815,7 @@
         <v>7</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C180" s="6" t="s">
         <v>31</v>
@@ -4868,7 +4838,7 @@
         <v>7</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C181" s="2" t="s">
         <v>31</v>
@@ -4891,7 +4861,7 @@
         <v>7</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C182" s="6" t="s">
         <v>42</v>
@@ -4914,7 +4884,7 @@
         <v>7</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C183" s="2" t="s">
         <v>42</v>
@@ -4937,7 +4907,7 @@
         <v>7</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C184" s="6" t="s">
         <v>42</v>
@@ -4960,7 +4930,7 @@
         <v>7</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>42</v>
@@ -4983,7 +4953,7 @@
         <v>7</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C186" s="6" t="s">
         <v>42</v>
@@ -5006,7 +4976,7 @@
         <v>7</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>49</v>
@@ -5029,7 +4999,7 @@
         <v>7</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C188" s="6" t="s">
         <v>49</v>
@@ -5052,7 +5022,7 @@
         <v>7</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>49</v>
@@ -5075,7 +5045,7 @@
         <v>7</v>
       </c>
       <c r="B190" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C190" s="6" t="s">
         <v>49</v>
@@ -5098,7 +5068,7 @@
         <v>7</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C191" s="2" t="s">
         <v>49</v>
@@ -5121,7 +5091,7 @@
         <v>7</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C192" s="6" t="s">
         <v>55</v>
@@ -5144,7 +5114,7 @@
         <v>7</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C193" s="2" t="s">
         <v>55</v>
@@ -5167,7 +5137,7 @@
         <v>7</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C194" s="6" t="s">
         <v>55</v>
@@ -5190,7 +5160,7 @@
         <v>7</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C195" s="2" t="s">
         <v>55</v>
@@ -5213,7 +5183,7 @@
         <v>7</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C196" s="6" t="s">
         <v>55</v>
@@ -5236,7 +5206,7 @@
         <v>7</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C197" s="2" t="s">
         <v>55</v>
@@ -5259,7 +5229,7 @@
         <v>7</v>
       </c>
       <c r="B198" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C198" s="6" t="s">
         <v>55</v>
@@ -5282,7 +5252,7 @@
         <v>7</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C199" s="2" t="s">
         <v>55</v>
@@ -5305,7 +5275,7 @@
         <v>7</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C200" s="6" t="s">
         <v>55</v>
@@ -5328,7 +5298,7 @@
         <v>7</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>55</v>
@@ -5351,7 +5321,7 @@
         <v>7</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C202" s="2" t="s">
         <v>62</v>
@@ -5374,7 +5344,7 @@
         <v>7</v>
       </c>
       <c r="B203" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C203" s="6" t="s">
         <v>62</v>
@@ -5397,7 +5367,7 @@
         <v>7</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C204" s="2" t="s">
         <v>62</v>
@@ -5420,7 +5390,7 @@
         <v>7</v>
       </c>
       <c r="B205" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C205" s="6" t="s">
         <v>62</v>
@@ -5443,7 +5413,7 @@
         <v>7</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C206" s="2" t="s">
         <v>62</v>
@@ -5466,7 +5436,7 @@
         <v>7</v>
       </c>
       <c r="B207" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C207" s="6" t="s">
         <v>62</v>
@@ -5489,7 +5459,7 @@
         <v>7</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C208" s="2" t="s">
         <v>62</v>
@@ -5512,7 +5482,7 @@
         <v>7</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C209" s="6" t="s">
         <v>62</v>
@@ -5521,7 +5491,7 @@
         <v>29</v>
       </c>
       <c r="E209" s="7" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F209" s="8" t="s">
         <v>12</v>
@@ -5535,7 +5505,7 @@
         <v>7</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C210" s="2" t="s">
         <v>73</v>
@@ -5558,7 +5528,7 @@
         <v>7</v>
       </c>
       <c r="B211" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C211" s="6" t="s">
         <v>73</v>
@@ -5581,7 +5551,7 @@
         <v>7</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C212" s="2" t="s">
         <v>73</v>
@@ -5604,7 +5574,7 @@
         <v>7</v>
       </c>
       <c r="B213" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C213" s="6" t="s">
         <v>73</v>
@@ -5627,7 +5597,7 @@
         <v>7</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C214" s="2" t="s">
         <v>73</v>
@@ -5650,7 +5620,7 @@
         <v>7</v>
       </c>
       <c r="B215" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C215" s="6" t="s">
         <v>9</v>
@@ -5659,7 +5629,7 @@
         <v>10</v>
       </c>
       <c r="E215" s="7" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F215" s="8" t="s">
         <v>12</v>
@@ -5673,7 +5643,7 @@
         <v>7</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C216" s="2" t="s">
         <v>9</v>
@@ -5696,7 +5666,7 @@
         <v>7</v>
       </c>
       <c r="B217" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C217" s="6" t="s">
         <v>9</v>
@@ -5719,7 +5689,7 @@
         <v>7</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C218" s="2" t="s">
         <v>9</v>
@@ -5742,7 +5712,7 @@
         <v>7</v>
       </c>
       <c r="B219" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C219" s="6" t="s">
         <v>9</v>
@@ -5765,7 +5735,7 @@
         <v>7</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C220" s="2" t="s">
         <v>9</v>
@@ -5774,7 +5744,7 @@
         <v>21</v>
       </c>
       <c r="E220" s="3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="F220" s="4" t="s">
         <v>12</v>
@@ -5788,7 +5758,7 @@
         <v>7</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C221" s="6" t="s">
         <v>9</v>
@@ -5811,7 +5781,7 @@
         <v>7</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C222" s="2" t="s">
         <v>9</v>
@@ -5834,7 +5804,7 @@
         <v>7</v>
       </c>
       <c r="B223" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C223" s="6" t="s">
         <v>9</v>
@@ -5857,7 +5827,7 @@
         <v>7</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C224" s="2" t="s">
         <v>9</v>
@@ -5880,7 +5850,7 @@
         <v>7</v>
       </c>
       <c r="B225" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C225" s="6" t="s">
         <v>31</v>
@@ -5903,7 +5873,7 @@
         <v>7</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C226" s="2" t="s">
         <v>31</v>
@@ -5926,7 +5896,7 @@
         <v>7</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C227" s="6" t="s">
         <v>31</v>
@@ -5949,7 +5919,7 @@
         <v>7</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C228" s="2" t="s">
         <v>31</v>
@@ -5972,7 +5942,7 @@
         <v>7</v>
       </c>
       <c r="B229" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C229" s="6" t="s">
         <v>31</v>
@@ -5995,7 +5965,7 @@
         <v>7</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C230" s="2" t="s">
         <v>31</v>
@@ -6018,7 +5988,7 @@
         <v>7</v>
       </c>
       <c r="B231" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C231" s="6" t="s">
         <v>31</v>
@@ -6041,7 +6011,7 @@
         <v>7</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C232" s="2" t="s">
         <v>31</v>
@@ -6064,7 +6034,7 @@
         <v>7</v>
       </c>
       <c r="B233" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C233" s="6" t="s">
         <v>31</v>
@@ -6087,7 +6057,7 @@
         <v>7</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C234" s="2" t="s">
         <v>31</v>
@@ -6110,7 +6080,7 @@
         <v>7</v>
       </c>
       <c r="B235" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C235" s="6" t="s">
         <v>42</v>
@@ -6133,7 +6103,7 @@
         <v>7</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C236" s="2" t="s">
         <v>42</v>
@@ -6156,7 +6126,7 @@
         <v>7</v>
       </c>
       <c r="B237" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C237" s="6" t="s">
         <v>42</v>
@@ -6179,7 +6149,7 @@
         <v>7</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C238" s="2" t="s">
         <v>42</v>
@@ -6202,7 +6172,7 @@
         <v>7</v>
       </c>
       <c r="B239" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C239" s="6" t="s">
         <v>42</v>
@@ -6211,7 +6181,7 @@
         <v>5</v>
       </c>
       <c r="E239" s="7" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F239" s="8" t="s">
         <v>44</v>
@@ -6225,7 +6195,7 @@
         <v>7</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C240" s="2" t="s">
         <v>49</v>
@@ -6248,7 +6218,7 @@
         <v>7</v>
       </c>
       <c r="B241" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C241" s="6" t="s">
         <v>49</v>
@@ -6271,7 +6241,7 @@
         <v>7</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C242" s="2" t="s">
         <v>49</v>
@@ -6294,7 +6264,7 @@
         <v>7</v>
       </c>
       <c r="B243" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C243" s="6" t="s">
         <v>49</v>
@@ -6317,7 +6287,7 @@
         <v>7</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C244" s="2" t="s">
         <v>49</v>
@@ -6340,7 +6310,7 @@
         <v>7</v>
       </c>
       <c r="B245" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C245" s="6" t="s">
         <v>55</v>
@@ -6363,7 +6333,7 @@
         <v>7</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C246" s="2" t="s">
         <v>55</v>
@@ -6386,7 +6356,7 @@
         <v>7</v>
       </c>
       <c r="B247" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C247" s="6" t="s">
         <v>55</v>
@@ -6409,7 +6379,7 @@
         <v>7</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C248" s="2" t="s">
         <v>55</v>
@@ -6432,7 +6402,7 @@
         <v>7</v>
       </c>
       <c r="B249" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C249" s="6" t="s">
         <v>55</v>
@@ -6455,7 +6425,7 @@
         <v>7</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C250" s="2" t="s">
         <v>55</v>
@@ -6478,7 +6448,7 @@
         <v>7</v>
       </c>
       <c r="B251" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C251" s="6" t="s">
         <v>55</v>
@@ -6501,7 +6471,7 @@
         <v>7</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C252" s="2" t="s">
         <v>55</v>
@@ -6524,7 +6494,7 @@
         <v>7</v>
       </c>
       <c r="B253" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C253" s="6" t="s">
         <v>55</v>
@@ -6533,7 +6503,7 @@
         <v>29</v>
       </c>
       <c r="E253" s="7" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F253" s="8" t="s">
         <v>57</v>
@@ -6547,7 +6517,7 @@
         <v>7</v>
       </c>
       <c r="B254" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C254" s="6" t="s">
         <v>62</v>
@@ -6570,7 +6540,7 @@
         <v>7</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C255" s="2" t="s">
         <v>62</v>
@@ -6593,7 +6563,7 @@
         <v>7</v>
       </c>
       <c r="B256" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C256" s="6" t="s">
         <v>62</v>
@@ -6616,7 +6586,7 @@
         <v>7</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C257" s="2" t="s">
         <v>62</v>
@@ -6639,7 +6609,7 @@
         <v>7</v>
       </c>
       <c r="B258" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C258" s="6" t="s">
         <v>62</v>
@@ -6662,7 +6632,7 @@
         <v>7</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C259" s="2" t="s">
         <v>62</v>
@@ -6685,7 +6655,7 @@
         <v>7</v>
       </c>
       <c r="B260" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C260" s="6" t="s">
         <v>62</v>
@@ -6708,7 +6678,7 @@
         <v>7</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C261" s="2" t="s">
         <v>62</v>
@@ -6731,7 +6701,7 @@
         <v>7</v>
       </c>
       <c r="B262" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C262" s="6" t="s">
         <v>62</v>
@@ -6754,7 +6724,7 @@
         <v>7</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C263" s="2" t="s">
         <v>73</v>
@@ -6777,7 +6747,7 @@
         <v>7</v>
       </c>
       <c r="B264" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C264" s="6" t="s">
         <v>73</v>
@@ -6800,7 +6770,7 @@
         <v>7</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C265" s="2" t="s">
         <v>73</v>
@@ -6823,7 +6793,7 @@
         <v>7</v>
       </c>
       <c r="B266" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C266" s="6" t="s">
         <v>73</v>
@@ -6846,7 +6816,7 @@
         <v>7</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C267" s="2" t="s">
         <v>73</v>

</xml_diff>